<commit_message>
major changes on the active control files
</commit_message>
<xml_diff>
--- a/NameParts.xlsx
+++ b/NameParts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t xml:space="preserve">Motor </t>
   </si>
@@ -69,9 +69,6 @@
     <t>Lower body</t>
   </si>
   <si>
-    <t>Lower Body Tube</t>
-  </si>
-  <si>
     <t>Upper Body</t>
   </si>
   <si>
@@ -91,6 +88,36 @@
   </si>
   <si>
     <t>Avionics</t>
+  </si>
+  <si>
+    <t>Active control</t>
+  </si>
+  <si>
+    <t>Active control support</t>
+  </si>
+  <si>
+    <t>Brake</t>
+  </si>
+  <si>
+    <t>RORO2</t>
+  </si>
+  <si>
+    <t>Lower body tube</t>
+  </si>
+  <si>
+    <t>Servomotor</t>
+  </si>
+  <si>
+    <t>Brake Rod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screw Rod </t>
+  </si>
+  <si>
+    <t>Linear screw</t>
+  </si>
+  <si>
+    <t>Linear bolt</t>
   </si>
 </sst>
 </file>
@@ -114,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -123,6 +150,86 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -132,6 +239,97 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -141,10 +339,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H19"/>
+  <dimension ref="B3:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,167 +689,533 @@
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1100</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1101</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6">
+        <v>1102</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6">
+        <v>1103</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16">
+        <v>1104</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="12">
+        <v>1200</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1201</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6">
+        <v>1202</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6">
+        <v>1203</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16">
+        <v>1204</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6">
+        <v>1001</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="20"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16">
+        <v>1002</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="6">
+        <v>2100</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6">
+        <v>2200</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="8">
+        <v>3000</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>1000</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E22" s="9">
+        <v>3100</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
-        <v>1100</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E26" s="17">
+        <v>21100</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1">
-        <v>1101</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="G26" s="3">
+        <v>21101</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G8">
-        <v>1102</v>
-      </c>
-      <c r="H8" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6">
+        <v>21102</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G9">
-        <v>1103</v>
-      </c>
-      <c r="H9" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6">
+        <v>21103</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G10">
-        <v>1104</v>
-      </c>
-      <c r="H10" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16">
+        <v>21104</v>
+      </c>
+      <c r="H29" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E11">
-        <v>1200</v>
-      </c>
-      <c r="F11" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="12">
+        <v>21200</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G11">
-        <v>1201</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="G30" s="13">
+        <v>21201</v>
+      </c>
+      <c r="H30" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G12">
-        <v>1202</v>
-      </c>
-      <c r="H12" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6">
+        <v>21202</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G13">
-        <v>1203</v>
-      </c>
-      <c r="H13" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6">
+        <v>21203</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G14">
-        <v>1204</v>
-      </c>
-      <c r="H14" t="s">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16">
+        <v>21204</v>
+      </c>
+      <c r="H33" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G15">
-        <v>1001</v>
-      </c>
-      <c r="H15" t="s">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="12">
+        <v>21400</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="13">
+        <v>21401</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6">
+        <v>21402</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6">
+        <v>21403</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="21">
+        <v>21404</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="21">
+        <v>21405</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="21">
+        <v>21406</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="21">
+        <v>21407</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6">
+        <v>21001</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="20"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16">
+        <v>21002</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="5">
+        <v>22000</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G16">
-        <v>1002</v>
-      </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>2000</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E47" s="6">
+        <v>22100</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E17">
-        <v>2100</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="G47" s="6"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6">
+        <v>22200</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E18">
-        <v>2200</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>3000</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="G48" s="6"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="8">
+        <v>23000</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="9">
+        <v>23100</v>
+      </c>
+      <c r="F49" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E19">
-        <v>3100</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Major changes on active control, the fin assembly and tubes
</commit_message>
<xml_diff>
--- a/NameParts.xlsx
+++ b/NameParts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t xml:space="preserve">Motor </t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Linear bolt</t>
+  </si>
+  <si>
+    <t>Upper body tube</t>
   </si>
 </sst>
 </file>
@@ -676,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H49"/>
+  <dimension ref="B3:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,21 +1204,61 @@
       <c r="G48" s="6"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="8">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6">
+        <v>22001</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="5">
         <v>23000</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D51" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E51" s="6">
         <v>23100</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F51" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="10"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9">
+        <v>23001</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the CAD of the nosecone with the ejection system and right mass for CM (sorry the names are a bit messy)
</commit_message>
<xml_diff>
--- a/NameParts.xlsx
+++ b/NameParts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -681,26 +681,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
@@ -720,7 +720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>1000</v>
       </c>
@@ -740,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="14"/>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="14"/>
@@ -764,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="15"/>
@@ -776,7 +776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="12">
@@ -792,7 +792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="14"/>
@@ -804,7 +804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="14"/>
@@ -816,7 +816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="15"/>
@@ -828,7 +828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -836,7 +836,7 @@
       <c r="G15" s="6"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -844,7 +844,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -852,7 +852,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -864,7 +864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C19" s="20"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -876,7 +876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -892,7 +892,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6">
@@ -904,7 +904,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="8">
         <v>3000</v>
       </c>
@@ -920,8 +920,8 @@
       <c r="G22" s="9"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>26</v>
       </c>
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="14"/>
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="14"/>
@@ -968,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="15"/>
@@ -980,7 +980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="12">
@@ -996,7 +996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="14"/>
@@ -1008,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="14"/>
@@ -1020,7 +1020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="15"/>
@@ -1032,7 +1032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -1040,7 +1040,7 @@
       <c r="G34" s="6"/>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1048,7 +1048,7 @@
       <c r="G35" s="6"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="12">
@@ -1064,7 +1064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="14"/>
@@ -1076,7 +1076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
       <c r="E38" s="14"/>
@@ -1088,7 +1088,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="14"/>
@@ -1100,7 +1100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
       <c r="E40" s="14"/>
@@ -1112,7 +1112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="14"/>
@@ -1124,7 +1124,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="14"/>
@@ -1136,7 +1136,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
       <c r="E43" s="15"/>
@@ -1144,7 +1144,7 @@
       <c r="G43" s="16"/>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1152,7 +1152,7 @@
       <c r="G44" s="6"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1164,7 +1164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C46" s="20"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -1176,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C47" s="5">
         <v>22000</v>
       </c>
@@ -1192,7 +1192,7 @@
       <c r="G47" s="6"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6">
@@ -1204,7 +1204,7 @@
       <c r="G48" s="6"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C49" s="5"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -1216,7 +1216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C50" s="5"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -1224,7 +1224,7 @@
       <c r="G50" s="6"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C51" s="5">
         <v>23000</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="G51" s="6"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C52" s="5"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -1248,7 +1248,7 @@
       <c r="G52" s="6"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>

</xml_diff>